<commit_message>
Added credentials file and DataDrivenUser for manage it
</commit_message>
<xml_diff>
--- a/credentialsFile.xlsx
+++ b/credentialsFile.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId3" sheetId="1" state="visible"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>USERNAME</t>
   </si>
@@ -39,11 +41,15 @@
   <si>
     <t>uditeamacn4@gmail.com</t>
   </si>
+  <si>
+    <t>Success</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -79,32 +85,32 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -136,6 +142,9 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
Changes and Improvements with console messages
Bug with invalid email addres fixed.
Bug with NullPointerException after showing the singup screen fixed.
Bug with cycle for read accounts at end of the account list fixed.
Steps messages added for trace the execution.

NullPointerException catch on DataDrivenUser class for change the
control of cycle for read accounts.
</commit_message>
<xml_diff>
--- a/credentialsFile.xlsx
+++ b/credentialsFile.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="20">
   <si>
     <t>USERNAME</t>
   </si>
@@ -43,6 +43,36 @@
   </si>
   <si>
     <t>Success</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Fail: The password you entered is incorrect.</t>
+  </si>
+  <si>
+    <t>Fail: This account dont exist</t>
+  </si>
+  <si>
+    <t>Fail: [[AndroidDriver:  on LINUX (872ecd5b-06a1-42f0-9bc3-d3779ee1e9ac)] -&gt; id: com.pinterest:id/signup_name]</t>
+  </si>
+  <si>
+    <t>Fail: [[AndroidDriver:  on LINUX (b21e32bc-9611-4aed-bba3-2d20048e7630)] -&gt; id: com.pinterest:id/signup_name]</t>
+  </si>
+  <si>
+    <t>Fail: Hi, Cristian Camilo Isaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Login Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Login Fail: The password you entered is incorrect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Login Fail: Hi, Cristian Camilo Isaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Login Fail: Sorry this doesn't look like a valid email</t>
   </si>
 </sst>
 </file>
@@ -123,8 +153,8 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="C1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -134,6 +164,9 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -143,7 +176,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -153,6 +186,9 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -161,6 +197,9 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -168,6 +207,9 @@
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>